<commit_message>
Fixed opening and closing shift bug, adding serialization and deserialization of objects
</commit_message>
<xml_diff>
--- a/ExcelFiles/Offices/1.Admin Support.xlsx
+++ b/ExcelFiles/Offices/1.Admin Support.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Dropbox\Projects\ExcelParse\ExcelFiles\Offices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Dropbox\Projects\Scheduling Program\ExcelFiles\Offices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -553,7 +553,7 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -894,19 +894,19 @@
         <v>0.4375</v>
       </c>
       <c r="B12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -921,19 +921,19 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
@@ -951,13 +951,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
       </c>
       <c r="E14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -978,13 +978,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
       </c>
       <c r="E15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
@@ -1005,13 +1005,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
       </c>
       <c r="E16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
@@ -1032,13 +1032,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
@@ -1191,19 +1191,19 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="4">
         <v>0</v>
@@ -1218,19 +1218,19 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="4">
         <v>0</v>
@@ -1245,19 +1245,19 @@
         <v>0.70833333333333404</v>
       </c>
       <c r="B25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="4">
         <v>0</v>

</xml_diff>